<commit_message>
Generate User Input Excel sheet template based on projectionYear added.
</commit_message>
<xml_diff>
--- a/template/Template.xlsx
+++ b/template/Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ifinworth\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6973D088-2D74-4474-AE54-B618F4C9E1DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51AF97CF-6950-4D86-9E99-9D2CE8019A26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{11B12A5D-7249-4041-8AA7-3E354D49454B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{11B12A5D-7249-4041-8AA7-3E354D49454B}"/>
   </bookViews>
   <sheets>
     <sheet name="P&amp;L" sheetId="1" r:id="rId1"/>
@@ -348,7 +348,7 @@
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -429,6 +429,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -493,7 +501,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -561,6 +569,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="165" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -886,279 +900,281 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20D100AD-1EC3-3246-AFE5-16D06F619914}">
-  <dimension ref="A1:A58"/>
+  <dimension ref="A1:B58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="21.09765625" defaultRowHeight="25.2" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="57.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="53.09765625" customWidth="1"/>
+    <col min="2" max="2" width="33.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:2" s="25" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="26" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24"/>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="24"/>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B1" s="24"/>
+    </row>
+    <row r="2" spans="1:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="26"/>
+    </row>
+    <row r="3" spans="1:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="26"/>
+    </row>
+    <row r="4" spans="1:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
     </row>
-    <row r="25" spans="1:1" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="11" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="12" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="12" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="12" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="9"/>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="14" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="9"/>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="11" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="46" spans="1:1" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="15" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="15"/>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="12" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="12" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="13"/>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="9" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="13"/>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="11" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="13" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="13" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="13" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="13" t="s">
         <v>102</v>
       </c>
@@ -1168,6 +1184,7 @@
     <mergeCell ref="A1:A3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1175,345 +1192,346 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ABB34C2-FC5D-EB4C-A739-CF87FCBB2D79}">
   <dimension ref="A1:A72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="18.59765625" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="79.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.59765625" customWidth="1"/>
+    <col min="2" max="2" width="31.09765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:1" s="24" customFormat="1" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="27" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="25"/>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="25"/>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="27"/>
+    </row>
+    <row r="3" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="27"/>
+    </row>
+    <row r="4" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="17" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="17" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="17" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="17" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="17" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="17" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="17" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="17"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="18" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="18" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="18"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="16" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="19" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="17"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="19" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="17" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="17" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="17" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="17" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="17"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="16" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="17" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="17" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="17" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="17" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="17" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="17" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="17" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="20" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="17"/>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="16" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="16"/>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="18" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="21" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="16" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="22" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="22" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="22" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="22" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="22" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="22" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="22"/>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="22" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="23" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="17" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="17" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="19" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="17"/>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="18" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="19" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="19" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="19" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="19" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="23" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="23" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="23" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="19" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="17"/>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="17"/>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="20" t="s">
         <v>71</v>
       </c>

</xml_diff>

<commit_message>
header files font Calibri
</commit_message>
<xml_diff>
--- a/template/Template.xlsx
+++ b/template/Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shahnawaz/Documents/ifinworth/Project/ifinworth/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B291968-C13A-A446-8993-1114A2857CAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A89A9019-5A94-C349-8EBC-52BBE02A88F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17160" xr2:uid="{11B12A5D-7249-4041-8AA7-3E354D49454B}"/>
   </bookViews>
@@ -352,7 +352,7 @@
     <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -399,14 +399,6 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -420,11 +412,23 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -535,7 +539,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -564,7 +568,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -573,7 +577,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -605,27 +609,28 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="5" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="5" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -948,7 +953,7 @@
   <dimension ref="A1:BN58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection sqref="A1:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21.1640625" defaultRowHeight="25.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -957,8 +962,8 @@
     <col min="2" max="2" width="33.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:66" s="25" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:66" s="24" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="27" t="s">
         <v>101</v>
       </c>
       <c r="B1" s="26"/>
@@ -1027,8 +1032,8 @@
       <c r="BM1" s="26"/>
       <c r="BN1" s="26"/>
     </row>
-    <row r="2" spans="1:66" ht="25.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="27"/>
+    <row r="2" spans="1:66" s="25" customFormat="1" ht="25.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="28"/>
       <c r="B2" s="26"/>
       <c r="C2" s="26"/>
       <c r="D2" s="26"/>
@@ -1095,8 +1100,8 @@
       <c r="BM2" s="26"/>
       <c r="BN2" s="26"/>
     </row>
-    <row r="3" spans="1:66" ht="25.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="28"/>
+    <row r="3" spans="1:66" s="25" customFormat="1" ht="25.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="29"/>
       <c r="B3" s="26"/>
       <c r="C3" s="26"/>
       <c r="D3" s="26"/>
@@ -1497,7 +1502,7 @@
   <dimension ref="A1:BN72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection sqref="A1:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="18.6640625" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1506,7 +1511,7 @@
     <col min="2" max="2" width="31.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:66" s="24" customFormat="1" ht="40.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:66" s="31" customFormat="1" ht="40.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="30" t="s">
         <v>101</v>
       </c>
@@ -1576,8 +1581,8 @@
       <c r="BM1" s="26"/>
       <c r="BN1" s="26"/>
     </row>
-    <row r="2" spans="1:66" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="29"/>
+    <row r="2" spans="1:66" s="25" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="32"/>
       <c r="B2" s="26"/>
       <c r="C2" s="26"/>
       <c r="D2" s="26"/>
@@ -1644,8 +1649,8 @@
       <c r="BM2" s="26"/>
       <c r="BN2" s="26"/>
     </row>
-    <row r="3" spans="1:66" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="29"/>
+    <row r="3" spans="1:66" s="25" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="32"/>
       <c r="B3" s="26"/>
       <c r="C3" s="26"/>
       <c r="D3" s="26"/>

</xml_diff>